<commit_message>
Ajuste do erro nas fórmulas das células O119, O120 e O121 da aba "Relatório" e fórmulas O83 e O84 da aba "Estudo".
Signed-off-by: Jéfferson Pimenta Melo <jefferson.pimenta@hotmail.com>
</commit_message>
<xml_diff>
--- a/Análise de Risco.xlsx
+++ b/Análise de Risco.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" r:id="rId1"/>
@@ -1910,25 +1910,13 @@
     <xf numFmtId="11" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1937,7 +1925,28 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1955,16 +1964,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3194,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A226" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:S3"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A196" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="R207" sqref="R207:S207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3205,73 +3205,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3547,26 +3547,26 @@
       <c r="S17" s="16"/>
     </row>
     <row r="19" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
       <c r="S19" s="19"/>
     </row>
     <row r="20" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3601,13 +3601,13 @@
       <c r="S20" s="22"/>
     </row>
     <row r="21" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25" t="s">
         <v>123</v>
       </c>
       <c r="F21" s="22"/>
@@ -3633,12 +3633,12 @@
       <c r="Y21" s="3"/>
     </row>
     <row r="22" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="22" t="s">
         <v>16</v>
       </c>
@@ -3657,18 +3657,18 @@
         <v>18.5</v>
       </c>
       <c r="P22" s="22"/>
-      <c r="Q22" s="29">
+      <c r="Q22" s="30">
         <f>O22*O23+2*(3*O24)*(O22+O23)+PI()*((3*O24)^2)</f>
         <v>7915.7694409323949</v>
       </c>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
     </row>
     <row r="23" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -3685,15 +3685,15 @@
         <v>8</v>
       </c>
       <c r="P23" s="22"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
     </row>
     <row r="24" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
@@ -3710,15 +3710,15 @@
         <v>14</v>
       </c>
       <c r="P24" s="22"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="29"/>
-      <c r="S24" s="29"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
     </row>
     <row r="25" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="22" t="s">
         <v>386</v>
       </c>
@@ -3737,17 +3737,17 @@
         <v>62</v>
       </c>
       <c r="P25" s="22"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
-      <c r="S25" s="29"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
     </row>
     <row r="26" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="22" t="s">
         <v>252</v>
       </c>
@@ -3838,23 +3838,23 @@
       <c r="S28" s="22"/>
     </row>
     <row r="29" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25" t="s">
         <v>377</v>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
       <c r="N29" s="19" t="s">
         <v>25</v>
       </c>
@@ -3869,19 +3869,19 @@
       <c r="S29" s="22"/>
     </row>
     <row r="30" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
       <c r="N30" s="19" t="s">
         <v>26</v>
       </c>
@@ -3894,10 +3894,10 @@
       <c r="S30" s="22"/>
     </row>
     <row r="31" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="22" t="s">
         <v>31</v>
       </c>
@@ -3924,10 +3924,10 @@
       <c r="S31" s="22"/>
     </row>
     <row r="32" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
       <c r="E32" s="22" t="s">
         <v>402</v>
       </c>
@@ -3954,27 +3954,27 @@
       <c r="S32" s="22"/>
     </row>
     <row r="34" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
     </row>
     <row r="35" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
@@ -4173,25 +4173,25 @@
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
       <c r="N41" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="O41" s="28" t="str">
+      <c r="O41" s="25" t="str">
         <f>VLOOKUP(E41,Dados!AI4:AO7,7,0)</f>
         <v>-</v>
       </c>
-      <c r="P41" s="28"/>
+      <c r="P41" s="25"/>
       <c r="Q41" s="22" t="s">
         <v>60</v>
       </c>
@@ -4199,23 +4199,23 @@
       <c r="S41" s="22"/>
     </row>
     <row r="42" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
       <c r="N42" s="19" t="s">
         <v>432</v>
       </c>
@@ -4231,19 +4231,19 @@
       <c r="S42" s="22"/>
     </row>
     <row r="43" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
       <c r="N43" s="19" t="s">
         <v>48</v>
       </c>
@@ -4339,23 +4339,23 @@
       <c r="S46" s="22"/>
     </row>
     <row r="47" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28" t="s">
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
       <c r="N47" s="19" t="s">
         <v>52</v>
       </c>
@@ -4371,23 +4371,23 @@
       <c r="S47" s="22"/>
     </row>
     <row r="48" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="27">
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="31">
         <v>6</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
       <c r="N48" s="19" t="s">
         <v>53</v>
       </c>
@@ -4403,27 +4403,27 @@
       <c r="S48" s="22"/>
     </row>
     <row r="49" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
       <c r="N49" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="O49" s="31">
+      <c r="O49" s="27">
         <f>1/O48</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P49" s="31"/>
+      <c r="P49" s="27"/>
       <c r="Q49" s="22" t="s">
         <v>63</v>
       </c>
@@ -4431,19 +4431,19 @@
       <c r="S49" s="22"/>
     </row>
     <row r="50" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
-      <c r="M50" s="27"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
       <c r="N50" s="19" t="s">
         <v>55</v>
       </c>
@@ -4459,25 +4459,25 @@
       <c r="S50" s="22"/>
     </row>
     <row r="51" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="32"/>
-      <c r="R51" s="32"/>
-      <c r="S51" s="32"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="28"/>
+      <c r="O51" s="28"/>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="28"/>
+      <c r="R51" s="28"/>
+      <c r="S51" s="28"/>
     </row>
     <row r="52" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
@@ -4645,25 +4645,25 @@
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
       <c r="N57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="O57" s="28" t="str">
+      <c r="O57" s="25" t="str">
         <f>VLOOKUP(E57,Dados!AI4:AO7,7,0)</f>
         <v>-</v>
       </c>
-      <c r="P57" s="28"/>
+      <c r="P57" s="25"/>
       <c r="Q57" s="22" t="s">
         <v>60</v>
       </c>
@@ -4671,23 +4671,23 @@
       <c r="S57" s="22"/>
     </row>
     <row r="58" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="25" t="s">
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="25"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
       <c r="N58" s="19" t="s">
         <v>485</v>
       </c>
@@ -4703,19 +4703,19 @@
       <c r="S58" s="22"/>
     </row>
     <row r="59" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="25"/>
-      <c r="J59" s="25"/>
-      <c r="K59" s="25"/>
-      <c r="L59" s="25"/>
-      <c r="M59" s="25"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
       <c r="N59" s="19" t="s">
         <v>48</v>
       </c>
@@ -4811,23 +4811,23 @@
       <c r="S62" s="22"/>
     </row>
     <row r="63" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28" t="s">
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-      <c r="J63" s="28"/>
-      <c r="K63" s="28"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="28"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="25"/>
+      <c r="K63" s="25"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
       <c r="N63" s="19" t="s">
         <v>52</v>
       </c>
@@ -4843,23 +4843,23 @@
       <c r="S63" s="22"/>
     </row>
     <row r="64" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="27">
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="31">
         <v>6</v>
       </c>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
-      <c r="K64" s="27"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
+      <c r="K64" s="31"/>
+      <c r="L64" s="31"/>
+      <c r="M64" s="31"/>
       <c r="N64" s="19" t="s">
         <v>53</v>
       </c>
@@ -4875,27 +4875,27 @@
       <c r="S64" s="22"/>
     </row>
     <row r="65" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="27"/>
-      <c r="K65" s="27"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="31"/>
+      <c r="L65" s="31"/>
+      <c r="M65" s="31"/>
       <c r="N65" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="O65" s="31">
+      <c r="O65" s="27">
         <f>1/O64</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P65" s="31"/>
+      <c r="P65" s="27"/>
       <c r="Q65" s="22" t="s">
         <v>63</v>
       </c>
@@ -4903,19 +4903,19 @@
       <c r="S65" s="22"/>
     </row>
     <row r="66" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="28"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="27"/>
-      <c r="K66" s="27"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="31"/>
+      <c r="K66" s="31"/>
+      <c r="L66" s="31"/>
+      <c r="M66" s="31"/>
       <c r="N66" s="19" t="s">
         <v>55</v>
       </c>
@@ -4952,27 +4952,27 @@
       <c r="S67" s="16"/>
     </row>
     <row r="68" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="26"/>
-      <c r="G68" s="26"/>
-      <c r="H68" s="26"/>
-      <c r="I68" s="26"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="26"/>
-      <c r="L68" s="26"/>
-      <c r="M68" s="26"/>
-      <c r="N68" s="26"/>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26"/>
-      <c r="Q68" s="26"/>
-      <c r="R68" s="26"/>
-      <c r="S68" s="26"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="24"/>
+      <c r="J68" s="24"/>
+      <c r="K68" s="24"/>
+      <c r="L68" s="24"/>
+      <c r="M68" s="24"/>
+      <c r="N68" s="24"/>
+      <c r="O68" s="24"/>
+      <c r="P68" s="24"/>
+      <c r="Q68" s="24"/>
+      <c r="R68" s="24"/>
+      <c r="S68" s="24"/>
     </row>
     <row r="69" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
@@ -5176,15 +5176,15 @@
       <c r="D75" s="22"/>
       <c r="E75" s="22"/>
       <c r="F75" s="22"/>
-      <c r="G75" s="25" t="s">
+      <c r="G75" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="H75" s="25"/>
-      <c r="I75" s="25"/>
-      <c r="J75" s="25"/>
-      <c r="K75" s="25"/>
-      <c r="L75" s="25"/>
-      <c r="M75" s="25"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="26"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="26"/>
       <c r="N75" s="19" t="s">
         <v>84</v>
       </c>
@@ -5242,15 +5242,15 @@
       <c r="D77" s="22"/>
       <c r="E77" s="22"/>
       <c r="F77" s="22"/>
-      <c r="G77" s="25" t="s">
+      <c r="G77" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="H77" s="25"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="25"/>
-      <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="25"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="26"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="26"/>
       <c r="N77" s="19" t="s">
         <v>433</v>
       </c>
@@ -5306,15 +5306,15 @@
       <c r="D79" s="22"/>
       <c r="E79" s="22"/>
       <c r="F79" s="22"/>
-      <c r="G79" s="25" t="s">
+      <c r="G79" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="H79" s="25"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="25"/>
-      <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="26"/>
+      <c r="L79" s="26"/>
+      <c r="M79" s="26"/>
       <c r="N79" s="19" t="s">
         <v>85</v>
       </c>
@@ -5330,27 +5330,27 @@
       <c r="S79" s="22"/>
     </row>
     <row r="81" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B81" s="26"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="26"/>
-      <c r="I81" s="26"/>
-      <c r="J81" s="26"/>
-      <c r="K81" s="26"/>
-      <c r="L81" s="26"/>
-      <c r="M81" s="26"/>
-      <c r="N81" s="26"/>
-      <c r="O81" s="26"/>
-      <c r="P81" s="26"/>
-      <c r="Q81" s="26"/>
-      <c r="R81" s="26"/>
-      <c r="S81" s="26"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+      <c r="N81" s="24"/>
+      <c r="O81" s="24"/>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="24"/>
+      <c r="R81" s="24"/>
+      <c r="S81" s="24"/>
     </row>
     <row r="82" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="22" t="s">
@@ -5583,21 +5583,21 @@
       <c r="S89" s="22"/>
     </row>
     <row r="90" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="25" t="s">
+      <c r="A90" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="25"/>
-      <c r="I90" s="25"/>
-      <c r="J90" s="25"/>
-      <c r="K90" s="25"/>
-      <c r="L90" s="25"/>
-      <c r="M90" s="25"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+      <c r="I90" s="26"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="26"/>
       <c r="N90" s="19" t="s">
         <v>113</v>
       </c>
@@ -5716,27 +5716,27 @@
       <c r="M94" s="17"/>
     </row>
     <row r="95" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="26" t="s">
+      <c r="A95" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="26"/>
-      <c r="H95" s="26"/>
-      <c r="I95" s="26"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="26"/>
-      <c r="L95" s="26"/>
-      <c r="M95" s="26"/>
-      <c r="N95" s="26"/>
-      <c r="O95" s="26"/>
-      <c r="P95" s="26"/>
-      <c r="Q95" s="26"/>
-      <c r="R95" s="26"/>
-      <c r="S95" s="26"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="24"/>
+      <c r="L95" s="24"/>
+      <c r="M95" s="24"/>
+      <c r="N95" s="24"/>
+      <c r="O95" s="24"/>
+      <c r="P95" s="24"/>
+      <c r="Q95" s="24"/>
+      <c r="R95" s="24"/>
+      <c r="S95" s="24"/>
     </row>
     <row r="96" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="22" t="s">
@@ -5892,27 +5892,27 @@
       <c r="S100" s="22"/>
     </row>
     <row r="102" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="26" t="s">
+      <c r="A102" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-      <c r="E102" s="26"/>
-      <c r="F102" s="26"/>
-      <c r="G102" s="26"/>
-      <c r="H102" s="26"/>
-      <c r="I102" s="26"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="26"/>
-      <c r="L102" s="26"/>
-      <c r="M102" s="26"/>
-      <c r="N102" s="26"/>
-      <c r="O102" s="26"/>
-      <c r="P102" s="26"/>
-      <c r="Q102" s="26"/>
-      <c r="R102" s="26"/>
-      <c r="S102" s="26"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24"/>
+      <c r="M102" s="24"/>
+      <c r="N102" s="24"/>
+      <c r="O102" s="24"/>
+      <c r="P102" s="24"/>
+      <c r="Q102" s="24"/>
+      <c r="R102" s="24"/>
+      <c r="S102" s="24"/>
     </row>
     <row r="103" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
@@ -6086,27 +6086,27 @@
       <c r="S108" s="16"/>
     </row>
     <row r="109" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="26" t="s">
+      <c r="A109" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="B109" s="26"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="26"/>
-      <c r="E109" s="26"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="26"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="26"/>
-      <c r="J109" s="26"/>
-      <c r="K109" s="26"/>
-      <c r="L109" s="26"/>
-      <c r="M109" s="26"/>
-      <c r="N109" s="26"/>
-      <c r="O109" s="26"/>
-      <c r="P109" s="26"/>
-      <c r="Q109" s="26"/>
-      <c r="R109" s="26"/>
-      <c r="S109" s="26"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+      <c r="I109" s="24"/>
+      <c r="J109" s="24"/>
+      <c r="K109" s="24"/>
+      <c r="L109" s="24"/>
+      <c r="M109" s="24"/>
+      <c r="N109" s="24"/>
+      <c r="O109" s="24"/>
+      <c r="P109" s="24"/>
+      <c r="Q109" s="24"/>
+      <c r="R109" s="24"/>
+      <c r="S109" s="24"/>
     </row>
     <row r="110" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
@@ -6394,7 +6394,7 @@
         <v>108</v>
       </c>
       <c r="O119" s="22">
-        <f>IFERROR(0,O70*O111*(O114/O118))</f>
+        <f>IFERROR(O70*O111*(O114/O118),0)</f>
         <v>0</v>
       </c>
       <c r="P119" s="22"/>
@@ -6424,7 +6424,7 @@
         <v>109</v>
       </c>
       <c r="O120" s="22">
-        <f>IFERROR(0,O74*O73*O79*O112*((O114+O115+O116+O117)/O118))</f>
+        <f>IFERROR(O74*O73*O79*O112*((O114+O115+O116+O117)/O118),0)</f>
         <v>0</v>
       </c>
       <c r="P120" s="22"/>
@@ -6454,7 +6454,7 @@
         <v>472</v>
       </c>
       <c r="O121" s="22">
-        <f>IFERROR(0,O113*(O117/O118))</f>
+        <f>IFERROR(O113*(O117/O118),0)</f>
         <v>0</v>
       </c>
       <c r="P121" s="22"/>
@@ -6465,27 +6465,27 @@
       <c r="S121" s="22"/>
     </row>
     <row r="123" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="26" t="s">
+      <c r="A123" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="26"/>
-      <c r="E123" s="26"/>
-      <c r="F123" s="26"/>
-      <c r="G123" s="26"/>
-      <c r="H123" s="26"/>
-      <c r="I123" s="26"/>
-      <c r="J123" s="26"/>
-      <c r="K123" s="26"/>
-      <c r="L123" s="26"/>
-      <c r="M123" s="26"/>
-      <c r="N123" s="26"/>
-      <c r="O123" s="26"/>
-      <c r="P123" s="26"/>
-      <c r="Q123" s="26"/>
-      <c r="R123" s="26"/>
-      <c r="S123" s="26"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="24"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="24"/>
+      <c r="L123" s="24"/>
+      <c r="M123" s="24"/>
+      <c r="N123" s="24"/>
+      <c r="O123" s="24"/>
+      <c r="P123" s="24"/>
+      <c r="Q123" s="24"/>
+      <c r="R123" s="24"/>
+      <c r="S123" s="24"/>
     </row>
     <row r="124" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
@@ -6786,27 +6786,27 @@
       <c r="S133" s="16"/>
     </row>
     <row r="134" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="26" t="s">
+      <c r="A134" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B134" s="26"/>
-      <c r="C134" s="26"/>
-      <c r="D134" s="26"/>
-      <c r="E134" s="26"/>
-      <c r="F134" s="26"/>
-      <c r="G134" s="26"/>
-      <c r="H134" s="26"/>
-      <c r="I134" s="26"/>
-      <c r="J134" s="26"/>
-      <c r="K134" s="26"/>
-      <c r="L134" s="26"/>
-      <c r="M134" s="26"/>
-      <c r="N134" s="26"/>
-      <c r="O134" s="26"/>
-      <c r="P134" s="26"/>
-      <c r="Q134" s="26"/>
-      <c r="R134" s="26"/>
-      <c r="S134" s="26"/>
+      <c r="B134" s="24"/>
+      <c r="C134" s="24"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="24"/>
+      <c r="F134" s="24"/>
+      <c r="G134" s="24"/>
+      <c r="H134" s="24"/>
+      <c r="I134" s="24"/>
+      <c r="J134" s="24"/>
+      <c r="K134" s="24"/>
+      <c r="L134" s="24"/>
+      <c r="M134" s="24"/>
+      <c r="N134" s="24"/>
+      <c r="O134" s="24"/>
+      <c r="P134" s="24"/>
+      <c r="Q134" s="24"/>
+      <c r="R134" s="24"/>
+      <c r="S134" s="24"/>
     </row>
     <row r="135" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="22" t="s">
@@ -7086,27 +7086,27 @@
       <c r="S143" s="22"/>
     </row>
     <row r="145" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="26" t="s">
+      <c r="A145" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="B145" s="26"/>
-      <c r="C145" s="26"/>
-      <c r="D145" s="26"/>
-      <c r="E145" s="26"/>
-      <c r="F145" s="26"/>
-      <c r="G145" s="26"/>
-      <c r="H145" s="26"/>
-      <c r="I145" s="26"/>
-      <c r="J145" s="26"/>
-      <c r="K145" s="26"/>
-      <c r="L145" s="26"/>
-      <c r="M145" s="26"/>
-      <c r="N145" s="26"/>
-      <c r="O145" s="26"/>
-      <c r="P145" s="26"/>
-      <c r="Q145" s="26"/>
-      <c r="R145" s="26"/>
-      <c r="S145" s="26"/>
+      <c r="B145" s="24"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="24"/>
+      <c r="G145" s="24"/>
+      <c r="H145" s="24"/>
+      <c r="I145" s="24"/>
+      <c r="J145" s="24"/>
+      <c r="K145" s="24"/>
+      <c r="L145" s="24"/>
+      <c r="M145" s="24"/>
+      <c r="N145" s="24"/>
+      <c r="O145" s="24"/>
+      <c r="P145" s="24"/>
+      <c r="Q145" s="24"/>
+      <c r="R145" s="24"/>
+      <c r="S145" s="24"/>
     </row>
     <row r="146" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="22" t="s">
@@ -7172,14 +7172,14 @@
       <c r="S147" s="22"/>
     </row>
     <row r="148" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="28" t="s">
+      <c r="A148" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="B148" s="28"/>
-      <c r="C148" s="28"/>
-      <c r="D148" s="28"/>
-      <c r="E148" s="28"/>
-      <c r="F148" s="28"/>
+      <c r="B148" s="25"/>
+      <c r="C148" s="25"/>
+      <c r="D148" s="25"/>
+      <c r="E148" s="25"/>
+      <c r="F148" s="25"/>
       <c r="G148" s="22" t="s">
         <v>71</v>
       </c>
@@ -7206,12 +7206,12 @@
       <c r="S148" s="22"/>
     </row>
     <row r="149" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="28"/>
-      <c r="B149" s="28"/>
-      <c r="C149" s="28"/>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
+      <c r="A149" s="25"/>
+      <c r="B149" s="25"/>
+      <c r="C149" s="25"/>
+      <c r="D149" s="25"/>
+      <c r="E149" s="25"/>
+      <c r="F149" s="25"/>
       <c r="G149" s="22" t="s">
         <v>72</v>
       </c>
@@ -7238,12 +7238,12 @@
       <c r="S149" s="22"/>
     </row>
     <row r="150" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="28"/>
-      <c r="B150" s="28"/>
-      <c r="C150" s="28"/>
-      <c r="D150" s="28"/>
-      <c r="E150" s="28"/>
-      <c r="F150" s="28"/>
+      <c r="A150" s="25"/>
+      <c r="B150" s="25"/>
+      <c r="C150" s="25"/>
+      <c r="D150" s="25"/>
+      <c r="E150" s="25"/>
+      <c r="F150" s="25"/>
       <c r="G150" s="22" t="s">
         <v>440</v>
       </c>
@@ -7270,14 +7270,14 @@
       <c r="S150" s="22"/>
     </row>
     <row r="151" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="28" t="s">
+      <c r="A151" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="B151" s="28"/>
-      <c r="C151" s="28"/>
-      <c r="D151" s="28"/>
-      <c r="E151" s="28"/>
-      <c r="F151" s="28"/>
+      <c r="B151" s="25"/>
+      <c r="C151" s="25"/>
+      <c r="D151" s="25"/>
+      <c r="E151" s="25"/>
+      <c r="F151" s="25"/>
       <c r="G151" s="22" t="s">
         <v>71</v>
       </c>
@@ -7304,12 +7304,12 @@
       <c r="S151" s="22"/>
     </row>
     <row r="152" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="28"/>
-      <c r="B152" s="28"/>
-      <c r="C152" s="28"/>
-      <c r="D152" s="28"/>
-      <c r="E152" s="28"/>
-      <c r="F152" s="28"/>
+      <c r="A152" s="25"/>
+      <c r="B152" s="25"/>
+      <c r="C152" s="25"/>
+      <c r="D152" s="25"/>
+      <c r="E152" s="25"/>
+      <c r="F152" s="25"/>
       <c r="G152" s="22" t="s">
         <v>72</v>
       </c>
@@ -7336,14 +7336,14 @@
       <c r="S152" s="22"/>
     </row>
     <row r="153" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="28" t="s">
+      <c r="A153" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="B153" s="28"/>
-      <c r="C153" s="28"/>
-      <c r="D153" s="28"/>
-      <c r="E153" s="28"/>
-      <c r="F153" s="28"/>
+      <c r="B153" s="25"/>
+      <c r="C153" s="25"/>
+      <c r="D153" s="25"/>
+      <c r="E153" s="25"/>
+      <c r="F153" s="25"/>
       <c r="G153" s="22" t="s">
         <v>71</v>
       </c>
@@ -7370,12 +7370,12 @@
       <c r="S153" s="22"/>
     </row>
     <row r="154" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="28"/>
-      <c r="B154" s="28"/>
-      <c r="C154" s="28"/>
-      <c r="D154" s="28"/>
-      <c r="E154" s="28"/>
-      <c r="F154" s="28"/>
+      <c r="A154" s="25"/>
+      <c r="B154" s="25"/>
+      <c r="C154" s="25"/>
+      <c r="D154" s="25"/>
+      <c r="E154" s="25"/>
+      <c r="F154" s="25"/>
       <c r="G154" s="22" t="s">
         <v>72</v>
       </c>
@@ -7402,14 +7402,14 @@
       <c r="S154" s="22"/>
     </row>
     <row r="155" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="28" t="s">
+      <c r="A155" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="B155" s="28"/>
-      <c r="C155" s="28"/>
-      <c r="D155" s="28"/>
-      <c r="E155" s="28"/>
-      <c r="F155" s="28"/>
+      <c r="B155" s="25"/>
+      <c r="C155" s="25"/>
+      <c r="D155" s="25"/>
+      <c r="E155" s="25"/>
+      <c r="F155" s="25"/>
       <c r="G155" s="22" t="s">
         <v>71</v>
       </c>
@@ -7436,12 +7436,12 @@
       <c r="S155" s="22"/>
     </row>
     <row r="156" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="28"/>
-      <c r="B156" s="28"/>
-      <c r="C156" s="28"/>
-      <c r="D156" s="28"/>
-      <c r="E156" s="28"/>
-      <c r="F156" s="28"/>
+      <c r="A156" s="25"/>
+      <c r="B156" s="25"/>
+      <c r="C156" s="25"/>
+      <c r="D156" s="25"/>
+      <c r="E156" s="25"/>
+      <c r="F156" s="25"/>
       <c r="G156" s="22" t="s">
         <v>72</v>
       </c>
@@ -7468,14 +7468,14 @@
       <c r="S156" s="22"/>
     </row>
     <row r="157" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="28" t="s">
+      <c r="A157" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="B157" s="28"/>
-      <c r="C157" s="28"/>
-      <c r="D157" s="28"/>
-      <c r="E157" s="28"/>
-      <c r="F157" s="28"/>
+      <c r="B157" s="25"/>
+      <c r="C157" s="25"/>
+      <c r="D157" s="25"/>
+      <c r="E157" s="25"/>
+      <c r="F157" s="25"/>
       <c r="G157" s="22" t="s">
         <v>71</v>
       </c>
@@ -7502,12 +7502,12 @@
       <c r="S157" s="22"/>
     </row>
     <row r="158" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="28"/>
-      <c r="B158" s="28"/>
-      <c r="C158" s="28"/>
-      <c r="D158" s="28"/>
-      <c r="E158" s="28"/>
-      <c r="F158" s="28"/>
+      <c r="A158" s="25"/>
+      <c r="B158" s="25"/>
+      <c r="C158" s="25"/>
+      <c r="D158" s="25"/>
+      <c r="E158" s="25"/>
+      <c r="F158" s="25"/>
       <c r="G158" s="22" t="s">
         <v>72</v>
       </c>
@@ -7534,14 +7534,14 @@
       <c r="S158" s="22"/>
     </row>
     <row r="159" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="28" t="s">
+      <c r="A159" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="B159" s="28"/>
-      <c r="C159" s="28"/>
-      <c r="D159" s="28"/>
-      <c r="E159" s="28"/>
-      <c r="F159" s="28"/>
+      <c r="B159" s="25"/>
+      <c r="C159" s="25"/>
+      <c r="D159" s="25"/>
+      <c r="E159" s="25"/>
+      <c r="F159" s="25"/>
       <c r="G159" s="22" t="s">
         <v>71</v>
       </c>
@@ -7568,12 +7568,12 @@
       <c r="S159" s="22"/>
     </row>
     <row r="160" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="28"/>
-      <c r="B160" s="28"/>
-      <c r="C160" s="28"/>
-      <c r="D160" s="28"/>
-      <c r="E160" s="28"/>
-      <c r="F160" s="28"/>
+      <c r="A160" s="25"/>
+      <c r="B160" s="25"/>
+      <c r="C160" s="25"/>
+      <c r="D160" s="25"/>
+      <c r="E160" s="25"/>
+      <c r="F160" s="25"/>
       <c r="G160" s="22" t="s">
         <v>72</v>
       </c>
@@ -7715,27 +7715,27 @@
       <c r="S164" s="18"/>
     </row>
     <row r="165" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="26" t="s">
+      <c r="A165" s="24" t="s">
         <v>512</v>
       </c>
-      <c r="B165" s="26"/>
-      <c r="C165" s="26"/>
-      <c r="D165" s="26"/>
-      <c r="E165" s="26"/>
-      <c r="F165" s="26"/>
-      <c r="G165" s="26"/>
-      <c r="H165" s="26"/>
-      <c r="I165" s="26"/>
-      <c r="J165" s="26"/>
-      <c r="K165" s="26"/>
-      <c r="L165" s="26"/>
-      <c r="M165" s="26"/>
-      <c r="N165" s="26"/>
-      <c r="O165" s="26"/>
-      <c r="P165" s="26"/>
-      <c r="Q165" s="26"/>
-      <c r="R165" s="26"/>
-      <c r="S165" s="26"/>
+      <c r="B165" s="24"/>
+      <c r="C165" s="24"/>
+      <c r="D165" s="24"/>
+      <c r="E165" s="24"/>
+      <c r="F165" s="24"/>
+      <c r="G165" s="24"/>
+      <c r="H165" s="24"/>
+      <c r="I165" s="24"/>
+      <c r="J165" s="24"/>
+      <c r="K165" s="24"/>
+      <c r="L165" s="24"/>
+      <c r="M165" s="24"/>
+      <c r="N165" s="24"/>
+      <c r="O165" s="24"/>
+      <c r="P165" s="24"/>
+      <c r="Q165" s="24"/>
+      <c r="R165" s="24"/>
+      <c r="S165" s="24"/>
     </row>
     <row r="166" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="22" t="s">
@@ -8284,27 +8284,27 @@
       <c r="S183"/>
     </row>
     <row r="184" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="26" t="s">
+      <c r="A184" s="24" t="s">
         <v>513</v>
       </c>
-      <c r="B184" s="26"/>
-      <c r="C184" s="26"/>
-      <c r="D184" s="26"/>
-      <c r="E184" s="26"/>
-      <c r="F184" s="26"/>
-      <c r="G184" s="26"/>
-      <c r="H184" s="26"/>
-      <c r="I184" s="26"/>
-      <c r="J184" s="26"/>
-      <c r="K184" s="26"/>
-      <c r="L184" s="26"/>
-      <c r="M184" s="26"/>
-      <c r="N184" s="26"/>
-      <c r="O184" s="26"/>
-      <c r="P184" s="26"/>
-      <c r="Q184" s="26"/>
-      <c r="R184" s="26"/>
-      <c r="S184" s="26"/>
+      <c r="B184" s="24"/>
+      <c r="C184" s="24"/>
+      <c r="D184" s="24"/>
+      <c r="E184" s="24"/>
+      <c r="F184" s="24"/>
+      <c r="G184" s="24"/>
+      <c r="H184" s="24"/>
+      <c r="I184" s="24"/>
+      <c r="J184" s="24"/>
+      <c r="K184" s="24"/>
+      <c r="L184" s="24"/>
+      <c r="M184" s="24"/>
+      <c r="N184" s="24"/>
+      <c r="O184" s="24"/>
+      <c r="P184" s="24"/>
+      <c r="Q184" s="24"/>
+      <c r="R184" s="24"/>
+      <c r="S184" s="24"/>
     </row>
     <row r="185" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="22" t="s">
@@ -8853,27 +8853,27 @@
       <c r="S202" s="16"/>
     </row>
     <row r="203" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="26" t="s">
+      <c r="A203" s="24" t="s">
         <v>514</v>
       </c>
-      <c r="B203" s="26"/>
-      <c r="C203" s="26"/>
-      <c r="D203" s="26"/>
-      <c r="E203" s="26"/>
-      <c r="F203" s="26"/>
-      <c r="G203" s="26"/>
-      <c r="H203" s="26"/>
-      <c r="I203" s="26"/>
-      <c r="J203" s="26"/>
-      <c r="K203" s="26"/>
-      <c r="L203" s="26"/>
-      <c r="M203" s="26"/>
-      <c r="N203" s="26"/>
-      <c r="O203" s="26"/>
-      <c r="P203" s="26"/>
-      <c r="Q203" s="26"/>
-      <c r="R203" s="26"/>
-      <c r="S203" s="26"/>
+      <c r="B203" s="24"/>
+      <c r="C203" s="24"/>
+      <c r="D203" s="24"/>
+      <c r="E203" s="24"/>
+      <c r="F203" s="24"/>
+      <c r="G203" s="24"/>
+      <c r="H203" s="24"/>
+      <c r="I203" s="24"/>
+      <c r="J203" s="24"/>
+      <c r="K203" s="24"/>
+      <c r="L203" s="24"/>
+      <c r="M203" s="24"/>
+      <c r="N203" s="24"/>
+      <c r="O203" s="24"/>
+      <c r="P203" s="24"/>
+      <c r="Q203" s="24"/>
+      <c r="R203" s="24"/>
+      <c r="S203" s="24"/>
     </row>
     <row r="204" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="22" t="s">
@@ -8899,12 +8899,12 @@
         <v>470</v>
       </c>
       <c r="M204" s="22"/>
-      <c r="N204" s="25" t="s">
+      <c r="N204" s="26" t="s">
         <v>511</v>
       </c>
-      <c r="O204" s="25"/>
-      <c r="P204" s="25"/>
-      <c r="Q204" s="25"/>
+      <c r="O204" s="26"/>
+      <c r="P204" s="26"/>
+      <c r="Q204" s="26"/>
       <c r="R204" s="22" t="s">
         <v>459</v>
       </c>
@@ -8931,10 +8931,10 @@
       </c>
       <c r="J205" s="22"/>
       <c r="K205" s="22"/>
-      <c r="L205" s="24">
+      <c r="L205" s="32">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M205" s="24"/>
+      <c r="M205" s="32"/>
       <c r="N205" s="22" t="s">
         <v>65</v>
       </c>
@@ -8966,16 +8966,16 @@
       </c>
       <c r="J206" s="22"/>
       <c r="K206" s="22"/>
-      <c r="L206" s="24">
+      <c r="L206" s="32">
         <v>1E-3</v>
       </c>
-      <c r="M206" s="24"/>
-      <c r="N206" s="25" t="s">
+      <c r="M206" s="32"/>
+      <c r="N206" s="26" t="s">
         <v>467</v>
       </c>
-      <c r="O206" s="25"/>
-      <c r="P206" s="25"/>
-      <c r="Q206" s="25"/>
+      <c r="O206" s="26"/>
+      <c r="P206" s="26"/>
+      <c r="Q206" s="26"/>
       <c r="R206" s="22" t="s">
         <v>459</v>
       </c>
@@ -9001,10 +9001,10 @@
       </c>
       <c r="J207" s="22"/>
       <c r="K207" s="22"/>
-      <c r="L207" s="24">
+      <c r="L207" s="32">
         <v>1E-4</v>
       </c>
-      <c r="M207" s="24"/>
+      <c r="M207" s="32"/>
       <c r="N207" s="22" t="s">
         <v>468</v>
       </c>
@@ -9037,10 +9037,10 @@
       </c>
       <c r="J208" s="22"/>
       <c r="K208" s="22"/>
-      <c r="L208" s="24">
+      <c r="L208" s="32">
         <v>1E-3</v>
       </c>
-      <c r="M208" s="24"/>
+      <c r="M208" s="32"/>
       <c r="N208" s="22" t="s">
         <v>469</v>
       </c>
@@ -9073,10 +9073,10 @@
       </c>
       <c r="J209" s="22"/>
       <c r="K209" s="22"/>
-      <c r="L209" s="24">
+      <c r="L209" s="32">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M209" s="24"/>
+      <c r="M209" s="32"/>
       <c r="N209" s="18"/>
       <c r="O209" s="18"/>
       <c r="P209" s="18"/>
@@ -9086,82 +9086,503 @@
     </row>
   </sheetData>
   <mergeCells count="597">
-    <mergeCell ref="A200:F200"/>
-    <mergeCell ref="G200:M200"/>
-    <mergeCell ref="O200:P200"/>
-    <mergeCell ref="Q200:S200"/>
-    <mergeCell ref="A201:M201"/>
-    <mergeCell ref="O201:P201"/>
-    <mergeCell ref="Q201:S201"/>
-    <mergeCell ref="A197:F197"/>
-    <mergeCell ref="G197:M197"/>
-    <mergeCell ref="O197:P197"/>
-    <mergeCell ref="Q197:S197"/>
-    <mergeCell ref="A198:M198"/>
-    <mergeCell ref="O198:P198"/>
-    <mergeCell ref="Q198:S198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="G199:M199"/>
-    <mergeCell ref="O199:P199"/>
-    <mergeCell ref="Q199:S199"/>
-    <mergeCell ref="A194:F194"/>
-    <mergeCell ref="G194:M194"/>
-    <mergeCell ref="O194:P194"/>
-    <mergeCell ref="Q194:S194"/>
-    <mergeCell ref="A195:M195"/>
-    <mergeCell ref="O195:P195"/>
-    <mergeCell ref="Q195:S195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="G196:M196"/>
-    <mergeCell ref="O196:P196"/>
-    <mergeCell ref="Q196:S196"/>
-    <mergeCell ref="A191:F191"/>
-    <mergeCell ref="G191:M191"/>
-    <mergeCell ref="O191:P191"/>
-    <mergeCell ref="Q191:S191"/>
-    <mergeCell ref="A192:M192"/>
-    <mergeCell ref="O192:P192"/>
-    <mergeCell ref="Q192:S192"/>
-    <mergeCell ref="A193:F193"/>
-    <mergeCell ref="G193:M193"/>
-    <mergeCell ref="O193:P193"/>
-    <mergeCell ref="Q193:S193"/>
-    <mergeCell ref="A188:M188"/>
-    <mergeCell ref="O188:P188"/>
-    <mergeCell ref="Q188:S188"/>
-    <mergeCell ref="A189:M189"/>
-    <mergeCell ref="O189:P189"/>
-    <mergeCell ref="Q189:S189"/>
-    <mergeCell ref="A190:F190"/>
-    <mergeCell ref="G190:M190"/>
-    <mergeCell ref="O190:P190"/>
-    <mergeCell ref="Q190:S190"/>
-    <mergeCell ref="A184:S184"/>
-    <mergeCell ref="A185:M185"/>
-    <mergeCell ref="O185:P185"/>
-    <mergeCell ref="Q185:S185"/>
-    <mergeCell ref="A186:M186"/>
-    <mergeCell ref="O186:P186"/>
-    <mergeCell ref="Q186:S186"/>
-    <mergeCell ref="A187:M187"/>
-    <mergeCell ref="O187:P187"/>
-    <mergeCell ref="Q187:S187"/>
-    <mergeCell ref="A203:S203"/>
-    <mergeCell ref="G204:H204"/>
-    <mergeCell ref="I204:K204"/>
-    <mergeCell ref="G205:H205"/>
-    <mergeCell ref="G206:H206"/>
-    <mergeCell ref="G207:H207"/>
-    <mergeCell ref="G208:H208"/>
-    <mergeCell ref="I205:K205"/>
-    <mergeCell ref="I206:K206"/>
-    <mergeCell ref="I207:K207"/>
-    <mergeCell ref="I208:K208"/>
-    <mergeCell ref="R204:S204"/>
-    <mergeCell ref="R205:S205"/>
-    <mergeCell ref="R206:S206"/>
-    <mergeCell ref="R207:S207"/>
-    <mergeCell ref="R208:S208"/>
+    <mergeCell ref="A209:E209"/>
+    <mergeCell ref="G209:H209"/>
+    <mergeCell ref="L209:M209"/>
+    <mergeCell ref="I209:K209"/>
+    <mergeCell ref="O113:P113"/>
+    <mergeCell ref="E110:M110"/>
+    <mergeCell ref="N204:Q204"/>
+    <mergeCell ref="N205:Q205"/>
+    <mergeCell ref="N206:Q206"/>
+    <mergeCell ref="N207:Q207"/>
+    <mergeCell ref="N208:Q208"/>
+    <mergeCell ref="A204:E204"/>
+    <mergeCell ref="A205:E205"/>
+    <mergeCell ref="A206:E206"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="L204:M204"/>
+    <mergeCell ref="L205:M205"/>
+    <mergeCell ref="L206:M206"/>
+    <mergeCell ref="L207:M207"/>
+    <mergeCell ref="L208:M208"/>
+    <mergeCell ref="O176:P176"/>
+    <mergeCell ref="O175:P175"/>
+    <mergeCell ref="O174:P174"/>
+    <mergeCell ref="Q86:S90"/>
+    <mergeCell ref="O93:P93"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="O63:P63"/>
+    <mergeCell ref="O79:P79"/>
+    <mergeCell ref="Q75:S75"/>
+    <mergeCell ref="Q76:S76"/>
+    <mergeCell ref="Q77:S77"/>
+    <mergeCell ref="Q78:S78"/>
+    <mergeCell ref="Q79:S79"/>
+    <mergeCell ref="O85:P85"/>
+    <mergeCell ref="O86:P86"/>
+    <mergeCell ref="Q82:S82"/>
+    <mergeCell ref="O82:P82"/>
+    <mergeCell ref="O83:P83"/>
+    <mergeCell ref="F96:M96"/>
+    <mergeCell ref="F97:M97"/>
+    <mergeCell ref="F98:M98"/>
+    <mergeCell ref="D103:M103"/>
+    <mergeCell ref="D104:M104"/>
+    <mergeCell ref="A109:S109"/>
+    <mergeCell ref="G172:M172"/>
+    <mergeCell ref="A173:M173"/>
+    <mergeCell ref="A171:F171"/>
+    <mergeCell ref="A172:F172"/>
+    <mergeCell ref="O172:P172"/>
+    <mergeCell ref="O171:P171"/>
+    <mergeCell ref="O169:P169"/>
+    <mergeCell ref="O170:P170"/>
+    <mergeCell ref="O168:P168"/>
+    <mergeCell ref="Q173:S173"/>
+    <mergeCell ref="Q169:S169"/>
+    <mergeCell ref="Q170:S170"/>
+    <mergeCell ref="Q171:S171"/>
+    <mergeCell ref="Q172:S172"/>
+    <mergeCell ref="G171:M171"/>
+    <mergeCell ref="O114:P114"/>
+    <mergeCell ref="Q111:S111"/>
+    <mergeCell ref="A119:C121"/>
+    <mergeCell ref="A182:M182"/>
+    <mergeCell ref="E48:M50"/>
+    <mergeCell ref="D120:M120"/>
+    <mergeCell ref="D121:M121"/>
+    <mergeCell ref="Q178:S178"/>
+    <mergeCell ref="Q179:S179"/>
+    <mergeCell ref="Q180:S180"/>
+    <mergeCell ref="Q181:S181"/>
+    <mergeCell ref="Q182:S182"/>
+    <mergeCell ref="O182:P182"/>
+    <mergeCell ref="O181:P181"/>
+    <mergeCell ref="O180:P180"/>
+    <mergeCell ref="O179:P179"/>
+    <mergeCell ref="O178:P178"/>
+    <mergeCell ref="Q163:S163"/>
+    <mergeCell ref="Q167:S167"/>
+    <mergeCell ref="Q168:S168"/>
+    <mergeCell ref="O173:P173"/>
+    <mergeCell ref="Q119:S119"/>
+    <mergeCell ref="Q120:S120"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="O117:P117"/>
+    <mergeCell ref="O110:P110"/>
+    <mergeCell ref="Q110:S110"/>
+    <mergeCell ref="D119:M119"/>
+    <mergeCell ref="O119:P119"/>
+    <mergeCell ref="G76:M76"/>
+    <mergeCell ref="G77:M77"/>
+    <mergeCell ref="G71:M71"/>
+    <mergeCell ref="G72:M72"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="E58:M59"/>
+    <mergeCell ref="E64:M66"/>
+    <mergeCell ref="G69:M69"/>
+    <mergeCell ref="G70:M70"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="A64:D66"/>
+    <mergeCell ref="A68:S68"/>
+    <mergeCell ref="O69:P69"/>
+    <mergeCell ref="Q69:S69"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="G74:M74"/>
+    <mergeCell ref="G75:M75"/>
+    <mergeCell ref="Q176:S176"/>
+    <mergeCell ref="Q177:S177"/>
+    <mergeCell ref="A180:F180"/>
+    <mergeCell ref="G174:M174"/>
+    <mergeCell ref="G175:M175"/>
+    <mergeCell ref="G177:M177"/>
+    <mergeCell ref="G178:M178"/>
+    <mergeCell ref="G180:M180"/>
+    <mergeCell ref="G181:M181"/>
+    <mergeCell ref="A176:M176"/>
+    <mergeCell ref="A179:M179"/>
+    <mergeCell ref="A174:F174"/>
+    <mergeCell ref="A175:F175"/>
+    <mergeCell ref="A177:F177"/>
+    <mergeCell ref="A178:F178"/>
+    <mergeCell ref="A181:F181"/>
+    <mergeCell ref="O177:P177"/>
+    <mergeCell ref="Q174:S174"/>
+    <mergeCell ref="Q175:S175"/>
+    <mergeCell ref="O163:P163"/>
+    <mergeCell ref="O162:P162"/>
+    <mergeCell ref="O167:P167"/>
+    <mergeCell ref="O161:P161"/>
+    <mergeCell ref="A165:S165"/>
+    <mergeCell ref="O166:P166"/>
+    <mergeCell ref="Q166:S166"/>
+    <mergeCell ref="A166:M166"/>
+    <mergeCell ref="G161:M161"/>
+    <mergeCell ref="G162:M162"/>
+    <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A162:F162"/>
+    <mergeCell ref="A170:M170"/>
+    <mergeCell ref="A169:M169"/>
+    <mergeCell ref="A168:M168"/>
+    <mergeCell ref="A167:M167"/>
+    <mergeCell ref="A163:M163"/>
+    <mergeCell ref="Q161:S161"/>
+    <mergeCell ref="Q162:S162"/>
+    <mergeCell ref="O155:P155"/>
+    <mergeCell ref="O156:P156"/>
+    <mergeCell ref="O157:P157"/>
+    <mergeCell ref="O158:P158"/>
+    <mergeCell ref="Q155:S155"/>
+    <mergeCell ref="Q156:S156"/>
+    <mergeCell ref="Q157:S157"/>
+    <mergeCell ref="Q158:S158"/>
+    <mergeCell ref="I160:M160"/>
+    <mergeCell ref="A155:F156"/>
+    <mergeCell ref="G155:H155"/>
+    <mergeCell ref="G156:H156"/>
+    <mergeCell ref="A157:F158"/>
+    <mergeCell ref="G157:H157"/>
+    <mergeCell ref="G158:H158"/>
+    <mergeCell ref="I155:M155"/>
+    <mergeCell ref="I156:M156"/>
+    <mergeCell ref="I157:M157"/>
+    <mergeCell ref="I158:M158"/>
+    <mergeCell ref="Q151:S151"/>
+    <mergeCell ref="A151:F152"/>
+    <mergeCell ref="G151:H151"/>
+    <mergeCell ref="G152:H152"/>
+    <mergeCell ref="I151:M151"/>
+    <mergeCell ref="I152:M152"/>
+    <mergeCell ref="A153:F154"/>
+    <mergeCell ref="G153:H153"/>
+    <mergeCell ref="G154:H154"/>
+    <mergeCell ref="O151:P151"/>
+    <mergeCell ref="O152:P152"/>
+    <mergeCell ref="O153:P153"/>
+    <mergeCell ref="O154:P154"/>
+    <mergeCell ref="I153:M153"/>
+    <mergeCell ref="I154:M154"/>
+    <mergeCell ref="Q152:S152"/>
+    <mergeCell ref="Q153:S153"/>
+    <mergeCell ref="Q154:S154"/>
+    <mergeCell ref="A145:S145"/>
+    <mergeCell ref="Q146:S146"/>
+    <mergeCell ref="O146:P146"/>
+    <mergeCell ref="A146:H146"/>
+    <mergeCell ref="A147:H147"/>
+    <mergeCell ref="I146:M146"/>
+    <mergeCell ref="Q147:S147"/>
+    <mergeCell ref="Q148:S148"/>
+    <mergeCell ref="Q149:S149"/>
+    <mergeCell ref="A148:F150"/>
+    <mergeCell ref="G148:H148"/>
+    <mergeCell ref="G149:H149"/>
+    <mergeCell ref="G150:H150"/>
+    <mergeCell ref="Q150:S150"/>
+    <mergeCell ref="I147:M147"/>
+    <mergeCell ref="I148:M148"/>
+    <mergeCell ref="I149:M149"/>
+    <mergeCell ref="I150:M150"/>
+    <mergeCell ref="O147:P147"/>
+    <mergeCell ref="O148:P148"/>
+    <mergeCell ref="O149:P149"/>
+    <mergeCell ref="O150:P150"/>
+    <mergeCell ref="Q136:S136"/>
+    <mergeCell ref="Q137:S137"/>
+    <mergeCell ref="Q138:S138"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="Q140:S140"/>
+    <mergeCell ref="Q141:S141"/>
+    <mergeCell ref="Q142:S142"/>
+    <mergeCell ref="Q143:S143"/>
+    <mergeCell ref="D139:M139"/>
+    <mergeCell ref="D140:M140"/>
+    <mergeCell ref="D141:M141"/>
+    <mergeCell ref="D142:M142"/>
+    <mergeCell ref="D143:M143"/>
+    <mergeCell ref="A136:C137"/>
+    <mergeCell ref="A138:C140"/>
+    <mergeCell ref="A141:C143"/>
+    <mergeCell ref="D135:M135"/>
+    <mergeCell ref="D136:M136"/>
+    <mergeCell ref="D137:M137"/>
+    <mergeCell ref="D138:M138"/>
+    <mergeCell ref="O136:P136"/>
+    <mergeCell ref="O137:P137"/>
+    <mergeCell ref="O138:P138"/>
+    <mergeCell ref="O139:P139"/>
+    <mergeCell ref="O140:P140"/>
+    <mergeCell ref="O141:P141"/>
+    <mergeCell ref="O142:P142"/>
+    <mergeCell ref="O143:P143"/>
+    <mergeCell ref="Q127:S127"/>
+    <mergeCell ref="Q128:S128"/>
+    <mergeCell ref="Q129:S129"/>
+    <mergeCell ref="Q130:S130"/>
+    <mergeCell ref="Q131:S131"/>
+    <mergeCell ref="Q132:S132"/>
+    <mergeCell ref="D124:M124"/>
+    <mergeCell ref="A134:S134"/>
+    <mergeCell ref="Q135:S135"/>
+    <mergeCell ref="O135:P135"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="O124:P124"/>
+    <mergeCell ref="Q124:S124"/>
+    <mergeCell ref="A124:C124"/>
+    <mergeCell ref="A125:C126"/>
+    <mergeCell ref="A127:C129"/>
+    <mergeCell ref="A130:C132"/>
+    <mergeCell ref="D125:M125"/>
+    <mergeCell ref="D126:M126"/>
+    <mergeCell ref="D129:M129"/>
+    <mergeCell ref="D128:M128"/>
+    <mergeCell ref="D127:M127"/>
+    <mergeCell ref="D130:M130"/>
+    <mergeCell ref="D131:M131"/>
+    <mergeCell ref="D132:M132"/>
+    <mergeCell ref="O125:P125"/>
+    <mergeCell ref="O126:P126"/>
+    <mergeCell ref="O127:P127"/>
+    <mergeCell ref="O128:P128"/>
+    <mergeCell ref="O129:P129"/>
+    <mergeCell ref="O130:P130"/>
+    <mergeCell ref="O131:P131"/>
+    <mergeCell ref="O132:P132"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q125:S125"/>
+    <mergeCell ref="Q126:S126"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="A22:D25"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="E20:M20"/>
+    <mergeCell ref="E21:M21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E26:M26"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E2:S2"/>
+    <mergeCell ref="E3:S3"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="E22:M24"/>
+    <mergeCell ref="A19:R19"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="E29:M30"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q29:S30"/>
+    <mergeCell ref="E35:M35"/>
+    <mergeCell ref="A42:D43"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="E36:M36"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="E31:M31"/>
+    <mergeCell ref="E32:M32"/>
+    <mergeCell ref="A29:D32"/>
+    <mergeCell ref="A34:S34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A44:D46"/>
+    <mergeCell ref="A48:D50"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="E37:M37"/>
+    <mergeCell ref="E38:M38"/>
+    <mergeCell ref="E39:M39"/>
+    <mergeCell ref="E40:M40"/>
+    <mergeCell ref="E41:M41"/>
+    <mergeCell ref="E42:M43"/>
+    <mergeCell ref="E44:M46"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E47:M47"/>
+    <mergeCell ref="E52:M52"/>
+    <mergeCell ref="E53:M53"/>
+    <mergeCell ref="E54:M54"/>
+    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q40:S40"/>
+    <mergeCell ref="Q41:S41"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="Q42:S43"/>
+    <mergeCell ref="Q44:S46"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="O59:P59"/>
+    <mergeCell ref="O60:P60"/>
+    <mergeCell ref="Q63:S63"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="Q65:S65"/>
+    <mergeCell ref="Q66:S66"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="A51:S51"/>
+    <mergeCell ref="A58:D59"/>
+    <mergeCell ref="A60:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="O61:P61"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E55:M55"/>
+    <mergeCell ref="E56:M56"/>
+    <mergeCell ref="E57:M57"/>
+    <mergeCell ref="E63:M63"/>
+    <mergeCell ref="E60:M62"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="Q55:S55"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="O72:P72"/>
+    <mergeCell ref="O73:P73"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="O64:P64"/>
+    <mergeCell ref="O65:P65"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="O53:P53"/>
+    <mergeCell ref="O54:P54"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q58:S59"/>
+    <mergeCell ref="Q60:S62"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="Q71:S71"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="Q83:S85"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="Q72:S72"/>
+    <mergeCell ref="Q73:S73"/>
+    <mergeCell ref="Q74:S74"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="A77:B78"/>
+    <mergeCell ref="G73:M73"/>
+    <mergeCell ref="O78:P78"/>
+    <mergeCell ref="O75:P75"/>
+    <mergeCell ref="O76:P76"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="G83:M83"/>
+    <mergeCell ref="G84:M84"/>
+    <mergeCell ref="G85:M85"/>
+    <mergeCell ref="G78:M78"/>
+    <mergeCell ref="G79:M79"/>
+    <mergeCell ref="A82:M82"/>
+    <mergeCell ref="A79:F79"/>
+    <mergeCell ref="A95:S95"/>
+    <mergeCell ref="Q96:S96"/>
+    <mergeCell ref="O96:P96"/>
+    <mergeCell ref="E25:M25"/>
+    <mergeCell ref="A96:E96"/>
+    <mergeCell ref="O89:P89"/>
+    <mergeCell ref="O90:P90"/>
+    <mergeCell ref="O91:P91"/>
+    <mergeCell ref="O92:P92"/>
+    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="A92:M92"/>
+    <mergeCell ref="Q91:S91"/>
+    <mergeCell ref="Q92:S92"/>
+    <mergeCell ref="Q93:S93"/>
+    <mergeCell ref="A89:M89"/>
+    <mergeCell ref="A91:M91"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="A86:M86"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="A88:M88"/>
+    <mergeCell ref="O84:P84"/>
+    <mergeCell ref="O87:P87"/>
+    <mergeCell ref="O88:P88"/>
+    <mergeCell ref="A81:S81"/>
+    <mergeCell ref="O98:P98"/>
+    <mergeCell ref="O99:P99"/>
+    <mergeCell ref="O100:P100"/>
+    <mergeCell ref="A102:S102"/>
+    <mergeCell ref="Q103:S103"/>
+    <mergeCell ref="O103:P103"/>
+    <mergeCell ref="Q97:S98"/>
+    <mergeCell ref="Q99:S99"/>
+    <mergeCell ref="Q100:S100"/>
+    <mergeCell ref="A99:M99"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A97:E97"/>
+    <mergeCell ref="A98:E98"/>
+    <mergeCell ref="O97:P97"/>
+    <mergeCell ref="O106:P106"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="O120:P120"/>
+    <mergeCell ref="O121:P121"/>
+    <mergeCell ref="Q121:S121"/>
+    <mergeCell ref="A114:M114"/>
+    <mergeCell ref="A115:M115"/>
+    <mergeCell ref="O115:P115"/>
+    <mergeCell ref="Q112:S112"/>
+    <mergeCell ref="A116:M116"/>
+    <mergeCell ref="O116:P116"/>
+    <mergeCell ref="Q113:S113"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="O118:P118"/>
+    <mergeCell ref="Q114:S118"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="E111:M111"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="E112:M112"/>
+    <mergeCell ref="E113:M113"/>
+    <mergeCell ref="O111:P111"/>
+    <mergeCell ref="O112:P112"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="E28:M28"/>
     <mergeCell ref="O28:P28"/>
@@ -9186,503 +9607,82 @@
     <mergeCell ref="Q104:S104"/>
     <mergeCell ref="O104:P104"/>
     <mergeCell ref="O105:P105"/>
-    <mergeCell ref="O106:P106"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="O120:P120"/>
-    <mergeCell ref="O121:P121"/>
-    <mergeCell ref="Q121:S121"/>
-    <mergeCell ref="A114:M114"/>
-    <mergeCell ref="A115:M115"/>
-    <mergeCell ref="O115:P115"/>
-    <mergeCell ref="Q112:S112"/>
-    <mergeCell ref="A116:M116"/>
-    <mergeCell ref="O116:P116"/>
-    <mergeCell ref="Q113:S113"/>
-    <mergeCell ref="A118:M118"/>
-    <mergeCell ref="O118:P118"/>
-    <mergeCell ref="Q114:S118"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="E111:M111"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="E112:M112"/>
-    <mergeCell ref="E113:M113"/>
-    <mergeCell ref="O111:P111"/>
-    <mergeCell ref="O112:P112"/>
-    <mergeCell ref="O98:P98"/>
-    <mergeCell ref="O99:P99"/>
-    <mergeCell ref="O100:P100"/>
-    <mergeCell ref="A102:S102"/>
-    <mergeCell ref="Q103:S103"/>
-    <mergeCell ref="O103:P103"/>
-    <mergeCell ref="Q97:S98"/>
-    <mergeCell ref="Q99:S99"/>
-    <mergeCell ref="Q100:S100"/>
-    <mergeCell ref="A99:M99"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A97:E97"/>
-    <mergeCell ref="A98:E98"/>
-    <mergeCell ref="O97:P97"/>
-    <mergeCell ref="A95:S95"/>
-    <mergeCell ref="Q96:S96"/>
-    <mergeCell ref="O96:P96"/>
-    <mergeCell ref="E25:M25"/>
-    <mergeCell ref="A96:E96"/>
-    <mergeCell ref="O89:P89"/>
-    <mergeCell ref="O90:P90"/>
-    <mergeCell ref="O91:P91"/>
-    <mergeCell ref="O92:P92"/>
-    <mergeCell ref="A90:M90"/>
-    <mergeCell ref="A92:M92"/>
-    <mergeCell ref="Q91:S91"/>
-    <mergeCell ref="Q92:S92"/>
-    <mergeCell ref="Q93:S93"/>
-    <mergeCell ref="A89:M89"/>
-    <mergeCell ref="A91:M91"/>
-    <mergeCell ref="A93:M93"/>
-    <mergeCell ref="A86:M86"/>
-    <mergeCell ref="A87:M87"/>
-    <mergeCell ref="A88:M88"/>
-    <mergeCell ref="O84:P84"/>
-    <mergeCell ref="O87:P87"/>
-    <mergeCell ref="O88:P88"/>
-    <mergeCell ref="A81:S81"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="Q83:S85"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="Q72:S72"/>
-    <mergeCell ref="Q73:S73"/>
-    <mergeCell ref="Q74:S74"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="A75:B76"/>
-    <mergeCell ref="A77:B78"/>
-    <mergeCell ref="G73:M73"/>
-    <mergeCell ref="O78:P78"/>
-    <mergeCell ref="O75:P75"/>
-    <mergeCell ref="O76:P76"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="G83:M83"/>
-    <mergeCell ref="G84:M84"/>
-    <mergeCell ref="G85:M85"/>
-    <mergeCell ref="G78:M78"/>
-    <mergeCell ref="G79:M79"/>
-    <mergeCell ref="A82:M82"/>
-    <mergeCell ref="A79:F79"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="Q54:S54"/>
-    <mergeCell ref="Q55:S55"/>
-    <mergeCell ref="Q56:S56"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="O72:P72"/>
-    <mergeCell ref="O73:P73"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="O64:P64"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="O70:P70"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="O53:P53"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q58:S59"/>
-    <mergeCell ref="Q60:S62"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="Q71:S71"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="O59:P59"/>
-    <mergeCell ref="O60:P60"/>
-    <mergeCell ref="Q63:S63"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="Q65:S65"/>
-    <mergeCell ref="Q66:S66"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="Q50:S50"/>
-    <mergeCell ref="O49:P49"/>
-    <mergeCell ref="O50:P50"/>
-    <mergeCell ref="A51:S51"/>
-    <mergeCell ref="A58:D59"/>
-    <mergeCell ref="A60:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="O61:P61"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="E55:M55"/>
-    <mergeCell ref="E56:M56"/>
-    <mergeCell ref="E57:M57"/>
-    <mergeCell ref="E63:M63"/>
-    <mergeCell ref="E60:M62"/>
-    <mergeCell ref="Q47:S47"/>
-    <mergeCell ref="Q36:S36"/>
-    <mergeCell ref="Q37:S37"/>
-    <mergeCell ref="Q38:S38"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Q40:S40"/>
-    <mergeCell ref="Q41:S41"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q42:S43"/>
-    <mergeCell ref="Q44:S46"/>
-    <mergeCell ref="A44:D46"/>
-    <mergeCell ref="A48:D50"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="E37:M37"/>
-    <mergeCell ref="E38:M38"/>
-    <mergeCell ref="E39:M39"/>
-    <mergeCell ref="E40:M40"/>
-    <mergeCell ref="E41:M41"/>
-    <mergeCell ref="E42:M43"/>
-    <mergeCell ref="E44:M46"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E47:M47"/>
-    <mergeCell ref="E52:M52"/>
-    <mergeCell ref="E53:M53"/>
-    <mergeCell ref="E54:M54"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="E29:M30"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q29:S30"/>
-    <mergeCell ref="E35:M35"/>
-    <mergeCell ref="A42:D43"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="E36:M36"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="E31:M31"/>
-    <mergeCell ref="E32:M32"/>
-    <mergeCell ref="A29:D32"/>
-    <mergeCell ref="A34:S34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E2:S2"/>
-    <mergeCell ref="E3:S3"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="E22:M24"/>
-    <mergeCell ref="A19:R19"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q125:S125"/>
-    <mergeCell ref="Q126:S126"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="A22:D25"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="E20:M20"/>
-    <mergeCell ref="E21:M21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="Q22:S25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E26:M26"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="D132:M132"/>
-    <mergeCell ref="O125:P125"/>
-    <mergeCell ref="O126:P126"/>
-    <mergeCell ref="O127:P127"/>
-    <mergeCell ref="O128:P128"/>
-    <mergeCell ref="O129:P129"/>
-    <mergeCell ref="O130:P130"/>
-    <mergeCell ref="O131:P131"/>
-    <mergeCell ref="O132:P132"/>
-    <mergeCell ref="Q127:S127"/>
-    <mergeCell ref="Q128:S128"/>
-    <mergeCell ref="Q129:S129"/>
-    <mergeCell ref="Q130:S130"/>
-    <mergeCell ref="Q131:S131"/>
-    <mergeCell ref="Q132:S132"/>
-    <mergeCell ref="D124:M124"/>
-    <mergeCell ref="A134:S134"/>
-    <mergeCell ref="Q135:S135"/>
-    <mergeCell ref="O135:P135"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="O124:P124"/>
-    <mergeCell ref="Q124:S124"/>
-    <mergeCell ref="A124:C124"/>
-    <mergeCell ref="A125:C126"/>
-    <mergeCell ref="A127:C129"/>
-    <mergeCell ref="A130:C132"/>
-    <mergeCell ref="D125:M125"/>
-    <mergeCell ref="D126:M126"/>
-    <mergeCell ref="D129:M129"/>
-    <mergeCell ref="D128:M128"/>
-    <mergeCell ref="D127:M127"/>
-    <mergeCell ref="D130:M130"/>
-    <mergeCell ref="D131:M131"/>
-    <mergeCell ref="A136:C137"/>
-    <mergeCell ref="A138:C140"/>
-    <mergeCell ref="A141:C143"/>
-    <mergeCell ref="D135:M135"/>
-    <mergeCell ref="D136:M136"/>
-    <mergeCell ref="D137:M137"/>
-    <mergeCell ref="D138:M138"/>
-    <mergeCell ref="O136:P136"/>
-    <mergeCell ref="O137:P137"/>
-    <mergeCell ref="O138:P138"/>
-    <mergeCell ref="O139:P139"/>
-    <mergeCell ref="O140:P140"/>
-    <mergeCell ref="O141:P141"/>
-    <mergeCell ref="O142:P142"/>
-    <mergeCell ref="O143:P143"/>
-    <mergeCell ref="Q136:S136"/>
-    <mergeCell ref="Q137:S137"/>
-    <mergeCell ref="Q138:S138"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="Q140:S140"/>
-    <mergeCell ref="Q141:S141"/>
-    <mergeCell ref="Q142:S142"/>
-    <mergeCell ref="Q143:S143"/>
-    <mergeCell ref="D139:M139"/>
-    <mergeCell ref="D140:M140"/>
-    <mergeCell ref="D141:M141"/>
-    <mergeCell ref="D142:M142"/>
-    <mergeCell ref="D143:M143"/>
-    <mergeCell ref="A145:S145"/>
-    <mergeCell ref="Q146:S146"/>
-    <mergeCell ref="O146:P146"/>
-    <mergeCell ref="A146:H146"/>
-    <mergeCell ref="A147:H147"/>
-    <mergeCell ref="I146:M146"/>
-    <mergeCell ref="Q147:S147"/>
-    <mergeCell ref="Q148:S148"/>
-    <mergeCell ref="Q149:S149"/>
-    <mergeCell ref="A148:F150"/>
-    <mergeCell ref="G148:H148"/>
-    <mergeCell ref="G149:H149"/>
-    <mergeCell ref="G150:H150"/>
-    <mergeCell ref="Q150:S150"/>
-    <mergeCell ref="I147:M147"/>
-    <mergeCell ref="I148:M148"/>
-    <mergeCell ref="I149:M149"/>
-    <mergeCell ref="I150:M150"/>
-    <mergeCell ref="O147:P147"/>
-    <mergeCell ref="O148:P148"/>
-    <mergeCell ref="O149:P149"/>
-    <mergeCell ref="O150:P150"/>
-    <mergeCell ref="I157:M157"/>
-    <mergeCell ref="I158:M158"/>
-    <mergeCell ref="Q151:S151"/>
-    <mergeCell ref="A151:F152"/>
-    <mergeCell ref="G151:H151"/>
-    <mergeCell ref="G152:H152"/>
-    <mergeCell ref="I151:M151"/>
-    <mergeCell ref="I152:M152"/>
-    <mergeCell ref="A153:F154"/>
-    <mergeCell ref="G153:H153"/>
-    <mergeCell ref="G154:H154"/>
-    <mergeCell ref="O151:P151"/>
-    <mergeCell ref="O152:P152"/>
-    <mergeCell ref="O153:P153"/>
-    <mergeCell ref="O154:P154"/>
-    <mergeCell ref="I153:M153"/>
-    <mergeCell ref="I154:M154"/>
-    <mergeCell ref="Q152:S152"/>
-    <mergeCell ref="Q153:S153"/>
-    <mergeCell ref="Q154:S154"/>
-    <mergeCell ref="A170:M170"/>
-    <mergeCell ref="A169:M169"/>
-    <mergeCell ref="A168:M168"/>
-    <mergeCell ref="A167:M167"/>
-    <mergeCell ref="A163:M163"/>
-    <mergeCell ref="Q161:S161"/>
-    <mergeCell ref="Q162:S162"/>
-    <mergeCell ref="O155:P155"/>
-    <mergeCell ref="O156:P156"/>
-    <mergeCell ref="O157:P157"/>
-    <mergeCell ref="O158:P158"/>
-    <mergeCell ref="Q155:S155"/>
-    <mergeCell ref="Q156:S156"/>
-    <mergeCell ref="Q157:S157"/>
-    <mergeCell ref="Q158:S158"/>
-    <mergeCell ref="I160:M160"/>
-    <mergeCell ref="A155:F156"/>
-    <mergeCell ref="G155:H155"/>
-    <mergeCell ref="G156:H156"/>
-    <mergeCell ref="A157:F158"/>
-    <mergeCell ref="G157:H157"/>
-    <mergeCell ref="G158:H158"/>
-    <mergeCell ref="I155:M155"/>
-    <mergeCell ref="I156:M156"/>
-    <mergeCell ref="O163:P163"/>
-    <mergeCell ref="O162:P162"/>
-    <mergeCell ref="O167:P167"/>
-    <mergeCell ref="O161:P161"/>
-    <mergeCell ref="A165:S165"/>
-    <mergeCell ref="O166:P166"/>
-    <mergeCell ref="Q166:S166"/>
-    <mergeCell ref="A166:M166"/>
-    <mergeCell ref="G161:M161"/>
-    <mergeCell ref="G162:M162"/>
-    <mergeCell ref="A161:F161"/>
-    <mergeCell ref="A162:F162"/>
-    <mergeCell ref="Q176:S176"/>
-    <mergeCell ref="Q177:S177"/>
-    <mergeCell ref="A180:F180"/>
-    <mergeCell ref="G174:M174"/>
-    <mergeCell ref="G175:M175"/>
-    <mergeCell ref="G177:M177"/>
-    <mergeCell ref="G178:M178"/>
-    <mergeCell ref="G180:M180"/>
-    <mergeCell ref="G181:M181"/>
-    <mergeCell ref="A176:M176"/>
-    <mergeCell ref="A179:M179"/>
-    <mergeCell ref="A174:F174"/>
-    <mergeCell ref="A175:F175"/>
-    <mergeCell ref="A177:F177"/>
-    <mergeCell ref="A178:F178"/>
-    <mergeCell ref="A181:F181"/>
-    <mergeCell ref="O177:P177"/>
-    <mergeCell ref="Q174:S174"/>
-    <mergeCell ref="Q175:S175"/>
-    <mergeCell ref="D119:M119"/>
-    <mergeCell ref="O119:P119"/>
-    <mergeCell ref="G76:M76"/>
-    <mergeCell ref="G77:M77"/>
-    <mergeCell ref="G71:M71"/>
-    <mergeCell ref="G72:M72"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="E58:M59"/>
-    <mergeCell ref="E64:M66"/>
-    <mergeCell ref="G69:M69"/>
-    <mergeCell ref="G70:M70"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="A64:D66"/>
-    <mergeCell ref="A68:S68"/>
-    <mergeCell ref="O69:P69"/>
-    <mergeCell ref="Q69:S69"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="G74:M74"/>
-    <mergeCell ref="G75:M75"/>
-    <mergeCell ref="A182:M182"/>
-    <mergeCell ref="E48:M50"/>
-    <mergeCell ref="D120:M120"/>
-    <mergeCell ref="D121:M121"/>
-    <mergeCell ref="Q178:S178"/>
-    <mergeCell ref="Q179:S179"/>
-    <mergeCell ref="Q180:S180"/>
-    <mergeCell ref="Q181:S181"/>
-    <mergeCell ref="Q182:S182"/>
-    <mergeCell ref="O182:P182"/>
-    <mergeCell ref="O181:P181"/>
-    <mergeCell ref="O180:P180"/>
-    <mergeCell ref="O179:P179"/>
-    <mergeCell ref="O178:P178"/>
-    <mergeCell ref="Q163:S163"/>
-    <mergeCell ref="Q167:S167"/>
-    <mergeCell ref="Q168:S168"/>
-    <mergeCell ref="O173:P173"/>
-    <mergeCell ref="Q119:S119"/>
-    <mergeCell ref="Q120:S120"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="O117:P117"/>
-    <mergeCell ref="O110:P110"/>
-    <mergeCell ref="Q110:S110"/>
-    <mergeCell ref="F96:M96"/>
-    <mergeCell ref="F97:M97"/>
-    <mergeCell ref="F98:M98"/>
-    <mergeCell ref="D103:M103"/>
-    <mergeCell ref="D104:M104"/>
-    <mergeCell ref="A109:S109"/>
-    <mergeCell ref="G172:M172"/>
-    <mergeCell ref="A173:M173"/>
-    <mergeCell ref="A171:F171"/>
-    <mergeCell ref="A172:F172"/>
-    <mergeCell ref="O172:P172"/>
-    <mergeCell ref="O171:P171"/>
-    <mergeCell ref="O169:P169"/>
-    <mergeCell ref="O170:P170"/>
-    <mergeCell ref="O168:P168"/>
-    <mergeCell ref="Q173:S173"/>
-    <mergeCell ref="Q169:S169"/>
-    <mergeCell ref="Q170:S170"/>
-    <mergeCell ref="Q171:S171"/>
-    <mergeCell ref="Q172:S172"/>
-    <mergeCell ref="G171:M171"/>
-    <mergeCell ref="O114:P114"/>
-    <mergeCell ref="Q111:S111"/>
-    <mergeCell ref="A119:C121"/>
-    <mergeCell ref="Q86:S90"/>
-    <mergeCell ref="O93:P93"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="O63:P63"/>
-    <mergeCell ref="O79:P79"/>
-    <mergeCell ref="Q75:S75"/>
-    <mergeCell ref="Q76:S76"/>
-    <mergeCell ref="Q77:S77"/>
-    <mergeCell ref="Q78:S78"/>
-    <mergeCell ref="Q79:S79"/>
-    <mergeCell ref="O85:P85"/>
-    <mergeCell ref="O86:P86"/>
-    <mergeCell ref="Q82:S82"/>
-    <mergeCell ref="O82:P82"/>
-    <mergeCell ref="O83:P83"/>
-    <mergeCell ref="A209:E209"/>
-    <mergeCell ref="G209:H209"/>
-    <mergeCell ref="L209:M209"/>
-    <mergeCell ref="I209:K209"/>
-    <mergeCell ref="O113:P113"/>
-    <mergeCell ref="E110:M110"/>
-    <mergeCell ref="N204:Q204"/>
-    <mergeCell ref="N205:Q205"/>
-    <mergeCell ref="N206:Q206"/>
-    <mergeCell ref="N207:Q207"/>
-    <mergeCell ref="N208:Q208"/>
-    <mergeCell ref="A204:E204"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A206:E206"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="L204:M204"/>
-    <mergeCell ref="L205:M205"/>
-    <mergeCell ref="L206:M206"/>
-    <mergeCell ref="L207:M207"/>
-    <mergeCell ref="L208:M208"/>
-    <mergeCell ref="O176:P176"/>
-    <mergeCell ref="O175:P175"/>
-    <mergeCell ref="O174:P174"/>
+    <mergeCell ref="A203:S203"/>
+    <mergeCell ref="G204:H204"/>
+    <mergeCell ref="I204:K204"/>
+    <mergeCell ref="G205:H205"/>
+    <mergeCell ref="G206:H206"/>
+    <mergeCell ref="G207:H207"/>
+    <mergeCell ref="G208:H208"/>
+    <mergeCell ref="I205:K205"/>
+    <mergeCell ref="I206:K206"/>
+    <mergeCell ref="I207:K207"/>
+    <mergeCell ref="I208:K208"/>
+    <mergeCell ref="R204:S204"/>
+    <mergeCell ref="R205:S205"/>
+    <mergeCell ref="R206:S206"/>
+    <mergeCell ref="R207:S207"/>
+    <mergeCell ref="R208:S208"/>
+    <mergeCell ref="A184:S184"/>
+    <mergeCell ref="A185:M185"/>
+    <mergeCell ref="O185:P185"/>
+    <mergeCell ref="Q185:S185"/>
+    <mergeCell ref="A186:M186"/>
+    <mergeCell ref="O186:P186"/>
+    <mergeCell ref="Q186:S186"/>
+    <mergeCell ref="A187:M187"/>
+    <mergeCell ref="O187:P187"/>
+    <mergeCell ref="Q187:S187"/>
+    <mergeCell ref="A188:M188"/>
+    <mergeCell ref="O188:P188"/>
+    <mergeCell ref="Q188:S188"/>
+    <mergeCell ref="A189:M189"/>
+    <mergeCell ref="O189:P189"/>
+    <mergeCell ref="Q189:S189"/>
+    <mergeCell ref="A190:F190"/>
+    <mergeCell ref="G190:M190"/>
+    <mergeCell ref="O190:P190"/>
+    <mergeCell ref="Q190:S190"/>
+    <mergeCell ref="A191:F191"/>
+    <mergeCell ref="G191:M191"/>
+    <mergeCell ref="O191:P191"/>
+    <mergeCell ref="Q191:S191"/>
+    <mergeCell ref="A192:M192"/>
+    <mergeCell ref="O192:P192"/>
+    <mergeCell ref="Q192:S192"/>
+    <mergeCell ref="A193:F193"/>
+    <mergeCell ref="G193:M193"/>
+    <mergeCell ref="O193:P193"/>
+    <mergeCell ref="Q193:S193"/>
+    <mergeCell ref="A194:F194"/>
+    <mergeCell ref="G194:M194"/>
+    <mergeCell ref="O194:P194"/>
+    <mergeCell ref="Q194:S194"/>
+    <mergeCell ref="A195:M195"/>
+    <mergeCell ref="O195:P195"/>
+    <mergeCell ref="Q195:S195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="G196:M196"/>
+    <mergeCell ref="O196:P196"/>
+    <mergeCell ref="Q196:S196"/>
+    <mergeCell ref="A200:F200"/>
+    <mergeCell ref="G200:M200"/>
+    <mergeCell ref="O200:P200"/>
+    <mergeCell ref="Q200:S200"/>
+    <mergeCell ref="A201:M201"/>
+    <mergeCell ref="O201:P201"/>
+    <mergeCell ref="Q201:S201"/>
+    <mergeCell ref="A197:F197"/>
+    <mergeCell ref="G197:M197"/>
+    <mergeCell ref="O197:P197"/>
+    <mergeCell ref="Q197:S197"/>
+    <mergeCell ref="A198:M198"/>
+    <mergeCell ref="O198:P198"/>
+    <mergeCell ref="Q198:S198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="G199:M199"/>
+    <mergeCell ref="O199:P199"/>
+    <mergeCell ref="Q199:S199"/>
   </mergeCells>
   <conditionalFormatting sqref="G205:H205">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
@@ -9709,7 +9709,7 @@
       <formula>$L$205</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22:M24">
       <formula1>"Estudo com formato prismático simples,Estudo com formato prismático complexo"</formula1>
     </dataValidation>
@@ -9733,7 +9733,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="24">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="24">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Dados!$A$3:$A$6</xm:f>
@@ -9888,8 +9888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:S3"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O85" sqref="O85:P85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9898,73 +9898,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
     </row>
     <row r="8" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -10191,15 +10191,15 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
       <c r="N15" s="21" t="s">
         <v>84</v>
       </c>
@@ -10257,15 +10257,15 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="21" t="s">
         <v>433</v>
       </c>
@@ -10389,10 +10389,10 @@
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
-      <c r="L25" s="24">
+      <c r="L25" s="32">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M25" s="24"/>
+      <c r="M25" s="32"/>
       <c r="N25" s="22" t="str">
         <f>IF(G25&gt;L25,"Não","Sim")</f>
         <v>Sim</v>
@@ -10423,10 +10423,10 @@
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
-      <c r="L26" s="24">
+      <c r="L26" s="32">
         <v>1E-3</v>
       </c>
-      <c r="M26" s="24"/>
+      <c r="M26" s="32"/>
       <c r="N26" s="22" t="str">
         <f>IF(Relatório!R205="Sim",IF(G26&gt;L26,"Não","Sim"),"Não estudado")</f>
         <v>Sim</v>
@@ -10457,10 +10457,10 @@
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
-      <c r="L27" s="24">
+      <c r="L27" s="32">
         <v>1E-4</v>
       </c>
-      <c r="M27" s="24"/>
+      <c r="M27" s="32"/>
       <c r="N27" s="22" t="str">
         <f>IF(Relatório!R206="Sim",IF(G27&gt;L27,"Não","Sim"),"Não estudado")</f>
         <v>Não estudado</v>
@@ -10492,10 +10492,10 @@
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
-      <c r="L28" s="24">
+      <c r="L28" s="32">
         <v>1E-3</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="32"/>
       <c r="N28" s="22" t="str">
         <f>IF(Relatório!R208="Sim",IF(G28&gt;L28,"Não","Sim"),"Não estudado")</f>
         <v>Não estudado</v>
@@ -10593,14 +10593,14 @@
       <c r="S42" s="22"/>
     </row>
     <row r="43" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
       <c r="G43" s="22" t="s">
         <v>71</v>
       </c>
@@ -10627,12 +10627,12 @@
       <c r="S43" s="22"/>
     </row>
     <row r="44" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
       <c r="G44" s="22" t="s">
         <v>72</v>
       </c>
@@ -10659,12 +10659,12 @@
       <c r="S44" s="22"/>
     </row>
     <row r="45" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
       <c r="G45" s="22" t="s">
         <v>440</v>
       </c>
@@ -10691,14 +10691,14 @@
       <c r="S45" s="22"/>
     </row>
     <row r="46" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
       <c r="G46" s="22" t="s">
         <v>71</v>
       </c>
@@ -10725,12 +10725,12 @@
       <c r="S46" s="22"/>
     </row>
     <row r="47" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
       <c r="G47" s="22" t="s">
         <v>72</v>
       </c>
@@ -10757,14 +10757,14 @@
       <c r="S47" s="22"/>
     </row>
     <row r="48" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
       <c r="G48" s="22" t="s">
         <v>71</v>
       </c>
@@ -10791,12 +10791,12 @@
       <c r="S48" s="22"/>
     </row>
     <row r="49" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
       <c r="G49" s="22" t="s">
         <v>72</v>
       </c>
@@ -10823,14 +10823,14 @@
       <c r="S49" s="22"/>
     </row>
     <row r="50" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
       <c r="G50" s="22" t="s">
         <v>71</v>
       </c>
@@ -10857,12 +10857,12 @@
       <c r="S50" s="22"/>
     </row>
     <row r="51" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
       <c r="G51" s="22" t="s">
         <v>72</v>
       </c>
@@ -10889,14 +10889,14 @@
       <c r="S51" s="22"/>
     </row>
     <row r="52" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
       <c r="G52" s="22" t="s">
         <v>71</v>
       </c>
@@ -10923,12 +10923,12 @@
       <c r="S52" s="22"/>
     </row>
     <row r="53" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
       <c r="G53" s="22" t="s">
         <v>72</v>
       </c>
@@ -10955,14 +10955,14 @@
       <c r="S53" s="22"/>
     </row>
     <row r="54" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
       <c r="G54" s="22" t="s">
         <v>71</v>
       </c>
@@ -10989,12 +10989,12 @@
       <c r="S54" s="22"/>
     </row>
     <row r="55" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
       <c r="G55" s="22" t="s">
         <v>72</v>
       </c>
@@ -11794,7 +11794,7 @@
         <v>213</v>
       </c>
       <c r="O83" s="23">
-        <f>IF($R$24="Sim",Relatório!$O$136*$O$45*Relatório!O121,0)</f>
+        <f>IF(Relatório!R208="Sim",Relatório!$O$136*$O$45*Relatório!O121,0)</f>
         <v>0</v>
       </c>
       <c r="P83" s="23"/>
@@ -11824,7 +11824,7 @@
         <v>214</v>
       </c>
       <c r="O84" s="23">
-        <f>IF($R$24="Sim",Relatório!$O$137*$O$58*Relatório!O121,0)</f>
+        <f>IF(Relatório!R208="Sim",Relatório!$O$137*$O$58*Relatório!O121,0)</f>
         <v>0</v>
       </c>
       <c r="P84" s="23"/>
@@ -12212,6 +12212,254 @@
     </row>
   </sheetData>
   <mergeCells count="272">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:S3"/>
+    <mergeCell ref="A96:M96"/>
+    <mergeCell ref="O96:P96"/>
+    <mergeCell ref="Q96:S96"/>
+    <mergeCell ref="A94:F94"/>
+    <mergeCell ref="G94:M94"/>
+    <mergeCell ref="O94:P94"/>
+    <mergeCell ref="Q94:S94"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="G95:M95"/>
+    <mergeCell ref="O95:P95"/>
+    <mergeCell ref="Q95:S95"/>
+    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="G92:M92"/>
+    <mergeCell ref="O92:P92"/>
+    <mergeCell ref="Q92:S92"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="O93:P93"/>
+    <mergeCell ref="Q93:S93"/>
+    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="O90:P90"/>
+    <mergeCell ref="Q90:S90"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="G91:M91"/>
+    <mergeCell ref="O91:P91"/>
+    <mergeCell ref="Q91:S91"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="G88:M88"/>
+    <mergeCell ref="O88:P88"/>
+    <mergeCell ref="Q88:S88"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="G89:M89"/>
+    <mergeCell ref="O89:P89"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="G86:M86"/>
+    <mergeCell ref="O86:P86"/>
+    <mergeCell ref="Q86:S86"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="O87:P87"/>
+    <mergeCell ref="Q87:S87"/>
+    <mergeCell ref="A84:M84"/>
+    <mergeCell ref="O84:P84"/>
+    <mergeCell ref="Q84:S84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="G85:M85"/>
+    <mergeCell ref="O85:P85"/>
+    <mergeCell ref="Q85:S85"/>
+    <mergeCell ref="A82:M82"/>
+    <mergeCell ref="O82:P82"/>
+    <mergeCell ref="Q82:S82"/>
+    <mergeCell ref="A83:M83"/>
+    <mergeCell ref="O83:P83"/>
+    <mergeCell ref="Q83:S83"/>
+    <mergeCell ref="A81:M81"/>
+    <mergeCell ref="O81:P81"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="A8:S8"/>
+    <mergeCell ref="A79:S79"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:S26"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="A23:S23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="O80:P80"/>
+    <mergeCell ref="Q80:S80"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="G15:M15"/>
+    <mergeCell ref="G14:M14"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A46:F47"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:M46"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="G9:M9"/>
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="G11:M11"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="I42:M42"/>
+    <mergeCell ref="G16:M16"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="G18:M18"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="G76:M76"/>
+    <mergeCell ref="O76:P76"/>
+    <mergeCell ref="Q76:S76"/>
+    <mergeCell ref="A77:M77"/>
+    <mergeCell ref="O77:P77"/>
+    <mergeCell ref="Q77:S77"/>
+    <mergeCell ref="A74:M74"/>
+    <mergeCell ref="O74:P74"/>
+    <mergeCell ref="Q74:S74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="G75:M75"/>
+    <mergeCell ref="O75:P75"/>
+    <mergeCell ref="Q75:S75"/>
+    <mergeCell ref="G72:M72"/>
+    <mergeCell ref="O72:P72"/>
+    <mergeCell ref="Q72:S72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="G73:M73"/>
+    <mergeCell ref="O73:P73"/>
+    <mergeCell ref="Q73:S73"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="G70:M70"/>
+    <mergeCell ref="O70:P70"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="A71:M71"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="Q71:S71"/>
+    <mergeCell ref="O68:P68"/>
+    <mergeCell ref="Q68:S68"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="G69:M69"/>
+    <mergeCell ref="O69:P69"/>
+    <mergeCell ref="Q69:S69"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="G66:M66"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="Q66:S66"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="G67:M67"/>
+    <mergeCell ref="O67:P67"/>
+    <mergeCell ref="Q67:S67"/>
+    <mergeCell ref="A68:M68"/>
+    <mergeCell ref="O64:P64"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="A65:M65"/>
+    <mergeCell ref="O65:P65"/>
+    <mergeCell ref="Q65:S65"/>
+    <mergeCell ref="A62:M62"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="A63:M63"/>
+    <mergeCell ref="O63:P63"/>
+    <mergeCell ref="Q63:S63"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="O58:P58"/>
+    <mergeCell ref="Q58:S58"/>
+    <mergeCell ref="A60:S60"/>
+    <mergeCell ref="A61:M61"/>
+    <mergeCell ref="O61:P61"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="G56:M56"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="G57:M57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="A58:M58"/>
+    <mergeCell ref="O54:P54"/>
+    <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="I55:M55"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q55:S55"/>
+    <mergeCell ref="A52:F53"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:M52"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="I53:M53"/>
+    <mergeCell ref="O53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="A54:F55"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="I54:M54"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:M51"/>
+    <mergeCell ref="O51:P51"/>
+    <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="A48:F49"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:M49"/>
+    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="A50:F51"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:M50"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:M47"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="I44:M44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:M45"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:S45"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:F11"/>
@@ -12236,254 +12484,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="Q46:S46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:M47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q47:S47"/>
-    <mergeCell ref="I44:M44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:M45"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="O50:P50"/>
-    <mergeCell ref="Q50:S50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:M51"/>
-    <mergeCell ref="O51:P51"/>
-    <mergeCell ref="Q51:S51"/>
-    <mergeCell ref="A48:F49"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:M48"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:M49"/>
-    <mergeCell ref="O49:P49"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="A50:F51"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:M50"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="Q54:S54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="I55:M55"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q55:S55"/>
-    <mergeCell ref="A52:F53"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:M52"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I53:M53"/>
-    <mergeCell ref="O53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="A54:F55"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="I54:M54"/>
-    <mergeCell ref="O58:P58"/>
-    <mergeCell ref="Q58:S58"/>
-    <mergeCell ref="A60:S60"/>
-    <mergeCell ref="A61:M61"/>
-    <mergeCell ref="O61:P61"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="G56:M56"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="Q56:S56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="G57:M57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="O64:P64"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="A65:M65"/>
-    <mergeCell ref="O65:P65"/>
-    <mergeCell ref="Q65:S65"/>
-    <mergeCell ref="A62:M62"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="A63:M63"/>
-    <mergeCell ref="O63:P63"/>
-    <mergeCell ref="Q63:S63"/>
-    <mergeCell ref="A64:M64"/>
-    <mergeCell ref="O68:P68"/>
-    <mergeCell ref="Q68:S68"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="G69:M69"/>
-    <mergeCell ref="O69:P69"/>
-    <mergeCell ref="Q69:S69"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="G66:M66"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="Q66:S66"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="G67:M67"/>
-    <mergeCell ref="O67:P67"/>
-    <mergeCell ref="Q67:S67"/>
-    <mergeCell ref="A68:M68"/>
-    <mergeCell ref="G72:M72"/>
-    <mergeCell ref="O72:P72"/>
-    <mergeCell ref="Q72:S72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="G73:M73"/>
-    <mergeCell ref="O73:P73"/>
-    <mergeCell ref="Q73:S73"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="G70:M70"/>
-    <mergeCell ref="O70:P70"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="A71:M71"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="Q71:S71"/>
-    <mergeCell ref="G76:M76"/>
-    <mergeCell ref="O76:P76"/>
-    <mergeCell ref="Q76:S76"/>
-    <mergeCell ref="A77:M77"/>
-    <mergeCell ref="O77:P77"/>
-    <mergeCell ref="Q77:S77"/>
-    <mergeCell ref="A74:M74"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="Q74:S74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="G75:M75"/>
-    <mergeCell ref="O75:P75"/>
-    <mergeCell ref="Q75:S75"/>
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="I42:M42"/>
-    <mergeCell ref="G16:M16"/>
-    <mergeCell ref="G17:M17"/>
-    <mergeCell ref="G18:M18"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="G11:M11"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="A80:M80"/>
-    <mergeCell ref="O80:P80"/>
-    <mergeCell ref="Q80:S80"/>
-    <mergeCell ref="G13:M13"/>
-    <mergeCell ref="G15:M15"/>
-    <mergeCell ref="G14:M14"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A46:F47"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:M46"/>
-    <mergeCell ref="A8:S8"/>
-    <mergeCell ref="A79:S79"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:S26"/>
-    <mergeCell ref="N25:S25"/>
-    <mergeCell ref="A23:S23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="A82:M82"/>
-    <mergeCell ref="O82:P82"/>
-    <mergeCell ref="Q82:S82"/>
-    <mergeCell ref="A83:M83"/>
-    <mergeCell ref="O83:P83"/>
-    <mergeCell ref="Q83:S83"/>
-    <mergeCell ref="A81:M81"/>
-    <mergeCell ref="O81:P81"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="G86:M86"/>
-    <mergeCell ref="O86:P86"/>
-    <mergeCell ref="Q86:S86"/>
-    <mergeCell ref="A87:M87"/>
-    <mergeCell ref="O87:P87"/>
-    <mergeCell ref="Q87:S87"/>
-    <mergeCell ref="A84:M84"/>
-    <mergeCell ref="O84:P84"/>
-    <mergeCell ref="Q84:S84"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="G85:M85"/>
-    <mergeCell ref="O85:P85"/>
-    <mergeCell ref="Q85:S85"/>
-    <mergeCell ref="O90:P90"/>
-    <mergeCell ref="Q90:S90"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="G91:M91"/>
-    <mergeCell ref="O91:P91"/>
-    <mergeCell ref="Q91:S91"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="G88:M88"/>
-    <mergeCell ref="O88:P88"/>
-    <mergeCell ref="Q88:S88"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="G89:M89"/>
-    <mergeCell ref="O89:P89"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:S2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:S3"/>
-    <mergeCell ref="A96:M96"/>
-    <mergeCell ref="O96:P96"/>
-    <mergeCell ref="Q96:S96"/>
-    <mergeCell ref="A94:F94"/>
-    <mergeCell ref="G94:M94"/>
-    <mergeCell ref="O94:P94"/>
-    <mergeCell ref="Q94:S94"/>
-    <mergeCell ref="A95:F95"/>
-    <mergeCell ref="G95:M95"/>
-    <mergeCell ref="O95:P95"/>
-    <mergeCell ref="Q95:S95"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="G92:M92"/>
-    <mergeCell ref="O92:P92"/>
-    <mergeCell ref="Q92:S92"/>
-    <mergeCell ref="A93:M93"/>
-    <mergeCell ref="O93:P93"/>
-    <mergeCell ref="Q93:S93"/>
-    <mergeCell ref="A90:M90"/>
   </mergeCells>
   <conditionalFormatting sqref="G25:H25">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
@@ -12614,22 +12614,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="34"/>
       <c r="D1" s="6" t="s">
         <v>255</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="J1" s="42" t="s">
+      <c r="H1" s="36"/>
+      <c r="J1" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="K1" s="42"/>
+      <c r="K1" s="34"/>
       <c r="M1" s="33" t="s">
         <v>273</v>
       </c>
@@ -12659,33 +12659,33 @@
         <v>515</v>
       </c>
       <c r="AG1" s="33"/>
-      <c r="AI1" s="34" t="s">
+      <c r="AI1" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="35"/>
-      <c r="AO1" s="36"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="39"/>
       <c r="AP1" s="11"/>
-      <c r="AR1" s="34" t="s">
+      <c r="AR1" s="37" t="s">
         <v>331</v>
       </c>
-      <c r="AS1" s="35"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="35"/>
-      <c r="AV1" s="35"/>
-      <c r="AW1" s="36"/>
-      <c r="AY1" s="34" t="s">
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="39"/>
+      <c r="AY1" s="37" t="s">
         <v>336</v>
       </c>
-      <c r="AZ1" s="35"/>
-      <c r="BA1" s="36"/>
-      <c r="BC1" s="34" t="s">
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="39"/>
+      <c r="BC1" s="37" t="s">
         <v>346</v>
       </c>
-      <c r="BD1" s="36"/>
+      <c r="BD1" s="39"/>
       <c r="BF1" s="33" t="s">
         <v>352</v>
       </c>
@@ -12782,30 +12782,30 @@
       <c r="AG2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="42" t="s">
+      <c r="AI2" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="AJ2" s="42" t="s">
+      <c r="AJ2" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="AK2" s="42"/>
-      <c r="AL2" s="42"/>
-      <c r="AM2" s="42"/>
-      <c r="AN2" s="42"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
       <c r="AO2" s="7" t="s">
         <v>387</v>
       </c>
       <c r="AP2" s="12"/>
-      <c r="AR2" s="37" t="s">
+      <c r="AR2" s="40" t="s">
         <v>332</v>
       </c>
-      <c r="AS2" s="39" t="s">
+      <c r="AS2" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="AT2" s="40"/>
-      <c r="AU2" s="40"/>
-      <c r="AV2" s="40"/>
-      <c r="AW2" s="41"/>
+      <c r="AT2" s="42"/>
+      <c r="AU2" s="42"/>
+      <c r="AV2" s="42"/>
+      <c r="AW2" s="36"/>
       <c r="AY2" s="7" t="s">
         <v>94</v>
       </c>
@@ -12931,7 +12931,7 @@
       <c r="AG3" s="7">
         <v>1</v>
       </c>
-      <c r="AI3" s="42"/>
+      <c r="AI3" s="34"/>
       <c r="AJ3" s="7">
         <v>1</v>
       </c>
@@ -12949,7 +12949,7 @@
       </c>
       <c r="AO3" s="7"/>
       <c r="AP3" s="12"/>
-      <c r="AR3" s="38"/>
+      <c r="AR3" s="41"/>
       <c r="AS3" s="7">
         <v>1</v>
       </c>
@@ -12965,7 +12965,7 @@
       <c r="AW3" s="7">
         <v>6</v>
       </c>
-      <c r="AY3" s="42" t="s">
+      <c r="AY3" s="34" t="s">
         <v>337</v>
       </c>
       <c r="AZ3" s="6" t="s">
@@ -13132,7 +13132,7 @@
       <c r="AW4" s="7">
         <v>0.1</v>
       </c>
-      <c r="AY4" s="42"/>
+      <c r="AY4" s="34"/>
       <c r="AZ4" s="6" t="s">
         <v>339</v>
       </c>
@@ -13285,7 +13285,7 @@
       <c r="AW5" s="7">
         <v>0.04</v>
       </c>
-      <c r="AY5" s="42"/>
+      <c r="AY5" s="34"/>
       <c r="AZ5" s="6" t="s">
         <v>340</v>
       </c>
@@ -13414,7 +13414,7 @@
       <c r="AP6" s="12">
         <v>4</v>
       </c>
-      <c r="AY6" s="42"/>
+      <c r="AY6" s="34"/>
       <c r="AZ6" s="9" t="s">
         <v>341</v>
       </c>
@@ -13509,7 +13509,7 @@
       <c r="AP7" s="12">
         <v>5</v>
       </c>
-      <c r="AY7" s="42"/>
+      <c r="AY7" s="34"/>
       <c r="AZ7" s="9" t="s">
         <v>342</v>
       </c>
@@ -13560,7 +13560,7 @@
       <c r="X8" s="7">
         <v>0</v>
       </c>
-      <c r="AY8" s="42" t="s">
+      <c r="AY8" s="34" t="s">
         <v>343</v>
       </c>
       <c r="AZ8" s="9" t="s">
@@ -13595,7 +13595,7 @@
       <c r="X9" s="7">
         <v>0</v>
       </c>
-      <c r="AY9" s="42"/>
+      <c r="AY9" s="34"/>
       <c r="AZ9" s="6" t="s">
         <v>344</v>
       </c>
@@ -13628,7 +13628,7 @@
       <c r="X10" s="7">
         <v>0</v>
       </c>
-      <c r="AY10" s="42"/>
+      <c r="AY10" s="34"/>
       <c r="AZ10" s="6" t="s">
         <v>345</v>
       </c>
@@ -13685,21 +13685,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="AY8:AY10"/>
-    <mergeCell ref="AY1:BA1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AI1:AO1"/>
     <mergeCell ref="BU1:BW1"/>
     <mergeCell ref="BR1:BS1"/>
     <mergeCell ref="AR1:AW1"/>
@@ -13711,6 +13696,21 @@
     <mergeCell ref="BI1:BJ1"/>
     <mergeCell ref="BL1:BM1"/>
     <mergeCell ref="BO1:BP1"/>
+    <mergeCell ref="AY8:AY10"/>
+    <mergeCell ref="AY1:BA1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AJ2:AN2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AI1:AO1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>